<commit_message>
Added "Uses Javascript" and "Additional Comments" Column
</commit_message>
<xml_diff>
--- a/seller_list.xlsx
+++ b/seller_list.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\impudo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19160" yWindow="0" windowWidth="19160" windowHeight="23540" tabRatio="500"/>
+    <workbookView xWindow="19155" yWindow="0" windowWidth="19155" windowHeight="23535" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1580" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="450">
   <si>
     <t>Website</t>
   </si>
@@ -1345,6 +1350,33 @@
   </si>
   <si>
     <t>article class="post… portfolio" -&gt; ul class="prtfolio-content" -&gt; li</t>
+  </si>
+  <si>
+    <t>uses Javascript?</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>ul/li/a</t>
+  </si>
+  <si>
+    <t>Additional Comments</t>
+  </si>
+  <si>
+    <t>Also has a section "books and dvds". Should this be crawled too?</t>
+  </si>
+  <si>
+    <t>http://moderntimesberlin.com/achive/&lt;number&gt;.jpg and http://moderntimesberlin.com/weekly/&lt;number&gt;.jpg</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>http://www.mggalerie.com/en/collectionsen/</t>
+  </si>
+  <si>
+    <t>TODO</t>
   </si>
 </sst>
 </file>
@@ -1406,7 +1438,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1432,8 +1464,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1447,36 +1480,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="25"/>
   </cellXfs>
-  <cellStyles count="25">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="26">
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1802,28 +1845,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N373"/>
+  <dimension ref="A1:R373"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A332" workbookViewId="0">
+      <selection activeCell="A364" sqref="A364"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.75" customWidth="1"/>
+    <col min="4" max="4" width="33.875" customWidth="1"/>
+    <col min="5" max="5" width="14.25" customWidth="1"/>
+    <col min="6" max="6" width="30.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.125" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="Q1" t="s">
+        <v>441</v>
+      </c>
+      <c r="R1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1847,7 +1899,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1874,7 +1926,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1898,7 +1950,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1928,7 +1980,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1958,7 +2010,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1982,7 +2034,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -2012,7 +2064,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -2036,7 +2088,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -2060,7 +2112,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -2084,11 +2136,11 @@
         <v>370</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -2112,7 +2164,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -2136,7 +2188,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -2160,11 +2212,11 @@
         <v>372</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
@@ -2194,7 +2246,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
@@ -2224,7 +2276,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
@@ -2248,7 +2300,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -2272,7 +2324,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
@@ -2296,7 +2348,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
@@ -2320,7 +2372,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -2344,7 +2396,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
@@ -2368,7 +2420,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>22</v>
       </c>
@@ -2392,7 +2444,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
@@ -2416,7 +2468,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>413</v>
       </c>
@@ -2443,7 +2495,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>24</v>
       </c>
@@ -2467,7 +2519,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>25</v>
       </c>
@@ -2491,7 +2543,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>26</v>
       </c>
@@ -2515,7 +2567,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>27</v>
       </c>
@@ -2539,7 +2591,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>28</v>
       </c>
@@ -2563,7 +2615,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>29</v>
       </c>
@@ -2587,7 +2639,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>30</v>
       </c>
@@ -2611,7 +2663,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>31</v>
       </c>
@@ -2635,7 +2687,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>32</v>
       </c>
@@ -2659,7 +2711,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>33</v>
       </c>
@@ -2683,7 +2735,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>34</v>
       </c>
@@ -2700,7 +2752,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>35</v>
       </c>
@@ -2724,7 +2776,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>36</v>
       </c>
@@ -2754,7 +2806,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>37</v>
       </c>
@@ -2769,7 +2821,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>38</v>
       </c>
@@ -2784,7 +2836,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>39</v>
       </c>
@@ -2799,7 +2851,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>40</v>
       </c>
@@ -2814,7 +2866,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>41</v>
       </c>
@@ -2829,7 +2881,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>42</v>
       </c>
@@ -2844,7 +2896,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>43</v>
       </c>
@@ -2859,7 +2911,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>44</v>
       </c>
@@ -2874,7 +2926,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>45</v>
       </c>
@@ -2889,7 +2941,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>46</v>
       </c>
@@ -2904,7 +2956,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>47</v>
       </c>
@@ -2919,7 +2971,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>48</v>
       </c>
@@ -2934,7 +2986,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>49</v>
       </c>
@@ -2949,7 +3001,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>50</v>
       </c>
@@ -2964,7 +3016,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>51</v>
       </c>
@@ -2979,7 +3031,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>52</v>
       </c>
@@ -2994,7 +3046,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>53</v>
       </c>
@@ -3009,7 +3061,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>54</v>
       </c>
@@ -3024,7 +3076,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>55</v>
       </c>
@@ -3039,7 +3091,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>56</v>
       </c>
@@ -3054,7 +3106,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>57</v>
       </c>
@@ -3069,7 +3121,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>58</v>
       </c>
@@ -3084,7 +3136,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>59</v>
       </c>
@@ -3099,7 +3151,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>60</v>
       </c>
@@ -3114,7 +3166,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>61</v>
       </c>
@@ -3129,7 +3181,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>62</v>
       </c>
@@ -3144,7 +3196,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>63</v>
       </c>
@@ -3159,7 +3211,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>64</v>
       </c>
@@ -3174,7 +3226,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>65</v>
       </c>
@@ -3189,7 +3241,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>66</v>
       </c>
@@ -3204,7 +3256,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>67</v>
       </c>
@@ -3219,7 +3271,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>68</v>
       </c>
@@ -3234,7 +3286,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>69</v>
       </c>
@@ -3249,7 +3301,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>70</v>
       </c>
@@ -3264,7 +3316,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>71</v>
       </c>
@@ -3279,7 +3331,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>72</v>
       </c>
@@ -3294,7 +3346,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>73</v>
       </c>
@@ -3309,7 +3361,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>74</v>
       </c>
@@ -3324,7 +3376,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>75</v>
       </c>
@@ -3339,7 +3391,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>76</v>
       </c>
@@ -3354,7 +3406,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>77</v>
       </c>
@@ -3369,7 +3421,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>78</v>
       </c>
@@ -3384,7 +3436,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>79</v>
       </c>
@@ -3399,7 +3451,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>80</v>
       </c>
@@ -3414,7 +3466,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>81</v>
       </c>
@@ -3429,7 +3481,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>82</v>
       </c>
@@ -3444,7 +3496,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>83</v>
       </c>
@@ -3459,7 +3511,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>84</v>
       </c>
@@ -3474,7 +3526,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>85</v>
       </c>
@@ -3489,7 +3541,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>86</v>
       </c>
@@ -3504,7 +3556,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>87</v>
       </c>
@@ -3519,7 +3571,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>88</v>
       </c>
@@ -3534,7 +3586,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>89</v>
       </c>
@@ -3549,7 +3601,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>90</v>
       </c>
@@ -3564,7 +3616,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>91</v>
       </c>
@@ -3579,7 +3631,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>92</v>
       </c>
@@ -3594,7 +3646,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>93</v>
       </c>
@@ -3609,7 +3661,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>94</v>
       </c>
@@ -3624,7 +3676,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>95</v>
       </c>
@@ -3639,7 +3691,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>96</v>
       </c>
@@ -3654,7 +3706,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>97</v>
       </c>
@@ -3669,7 +3721,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>98</v>
       </c>
@@ -3684,7 +3736,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>99</v>
       </c>
@@ -3699,7 +3751,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>100</v>
       </c>
@@ -3714,7 +3766,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>101</v>
       </c>
@@ -3729,7 +3781,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>102</v>
       </c>
@@ -3744,7 +3796,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>103</v>
       </c>
@@ -3759,7 +3811,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>104</v>
       </c>
@@ -3774,7 +3826,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>105</v>
       </c>
@@ -3789,7 +3841,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>106</v>
       </c>
@@ -3804,7 +3856,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>107</v>
       </c>
@@ -3819,7 +3871,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>108</v>
       </c>
@@ -3834,7 +3886,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>109</v>
       </c>
@@ -3849,7 +3901,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>110</v>
       </c>
@@ -3864,7 +3916,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>111</v>
       </c>
@@ -3879,7 +3931,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>112</v>
       </c>
@@ -3894,7 +3946,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>113</v>
       </c>
@@ -3909,7 +3961,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>114</v>
       </c>
@@ -3924,7 +3976,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>115</v>
       </c>
@@ -3939,7 +3991,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>116</v>
       </c>
@@ -3954,7 +4006,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>117</v>
       </c>
@@ -3969,7 +4021,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>118</v>
       </c>
@@ -3984,7 +4036,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>119</v>
       </c>
@@ -3999,7 +4051,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>120</v>
       </c>
@@ -4014,7 +4066,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>121</v>
       </c>
@@ -4029,7 +4081,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>122</v>
       </c>
@@ -4044,7 +4096,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>123</v>
       </c>
@@ -4059,7 +4111,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>124</v>
       </c>
@@ -4074,7 +4126,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>125</v>
       </c>
@@ -4089,7 +4141,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>126</v>
       </c>
@@ -4104,7 +4156,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>127</v>
       </c>
@@ -4119,7 +4171,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>128</v>
       </c>
@@ -4134,7 +4186,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>129</v>
       </c>
@@ -4149,7 +4201,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>130</v>
       </c>
@@ -4164,7 +4216,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>131</v>
       </c>
@@ -4179,7 +4231,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>132</v>
       </c>
@@ -4194,7 +4246,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>133</v>
       </c>
@@ -4209,7 +4261,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>134</v>
       </c>
@@ -4224,7 +4276,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>135</v>
       </c>
@@ -4239,7 +4291,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>136</v>
       </c>
@@ -4254,7 +4306,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>137</v>
       </c>
@@ -4269,7 +4321,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>138</v>
       </c>
@@ -4284,7 +4336,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>139</v>
       </c>
@@ -4299,7 +4351,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>140</v>
       </c>
@@ -4314,7 +4366,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="145" spans="1:7">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>141</v>
       </c>
@@ -4329,7 +4381,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>142</v>
       </c>
@@ -4344,7 +4396,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>143</v>
       </c>
@@ -4359,7 +4411,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>144</v>
       </c>
@@ -4374,7 +4426,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>145</v>
       </c>
@@ -4389,7 +4441,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>146</v>
       </c>
@@ -4404,7 +4456,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>147</v>
       </c>
@@ -4419,7 +4471,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>148</v>
       </c>
@@ -4434,7 +4486,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>149</v>
       </c>
@@ -4449,7 +4501,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>150</v>
       </c>
@@ -4464,7 +4516,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>151</v>
       </c>
@@ -4479,7 +4531,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>152</v>
       </c>
@@ -4494,7 +4546,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>153</v>
       </c>
@@ -4509,7 +4561,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="158" spans="1:7">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>154</v>
       </c>
@@ -4524,7 +4576,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>155</v>
       </c>
@@ -4539,7 +4591,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="160" spans="1:7">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
         <v>156</v>
       </c>
@@ -4554,7 +4606,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>157</v>
       </c>
@@ -4569,7 +4621,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>158</v>
       </c>
@@ -4584,7 +4636,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
         <v>159</v>
       </c>
@@ -4599,7 +4651,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="164" spans="1:7">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
         <v>160</v>
       </c>
@@ -4614,7 +4666,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>161</v>
       </c>
@@ -4629,7 +4681,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="166" spans="1:7">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>162</v>
       </c>
@@ -4644,7 +4696,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="167" spans="1:7">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>163</v>
       </c>
@@ -4659,7 +4711,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="168" spans="1:7">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>164</v>
       </c>
@@ -4674,7 +4726,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="169" spans="1:7">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
         <v>165</v>
       </c>
@@ -4689,7 +4741,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="170" spans="1:7">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
         <v>166</v>
       </c>
@@ -4704,7 +4756,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="171" spans="1:7">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
         <v>167</v>
       </c>
@@ -4719,7 +4771,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="172" spans="1:7">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
         <v>168</v>
       </c>
@@ -4734,7 +4786,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="173" spans="1:7">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
         <v>169</v>
       </c>
@@ -4749,7 +4801,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="174" spans="1:7">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
         <v>170</v>
       </c>
@@ -4764,7 +4816,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="175" spans="1:7">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
         <v>171</v>
       </c>
@@ -4779,7 +4831,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="176" spans="1:7">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
         <v>172</v>
       </c>
@@ -4794,7 +4846,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="177" spans="1:7">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
         <v>173</v>
       </c>
@@ -4809,7 +4861,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="178" spans="1:7">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
         <v>174</v>
       </c>
@@ -4824,7 +4876,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="179" spans="1:7">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
         <v>175</v>
       </c>
@@ -4839,7 +4891,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="180" spans="1:7">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
         <v>176</v>
       </c>
@@ -4854,7 +4906,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="181" spans="1:7">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
         <v>177</v>
       </c>
@@ -4869,7 +4921,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="182" spans="1:7">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
         <v>178</v>
       </c>
@@ -4884,7 +4936,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="183" spans="1:7">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
         <v>179</v>
       </c>
@@ -4899,7 +4951,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="184" spans="1:7">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
         <v>180</v>
       </c>
@@ -4914,7 +4966,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="185" spans="1:7">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
         <v>181</v>
       </c>
@@ -4929,7 +4981,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="186" spans="1:7">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
         <v>182</v>
       </c>
@@ -4944,7 +4996,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="187" spans="1:7">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
         <v>183</v>
       </c>
@@ -4959,7 +5011,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="188" spans="1:7">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
         <v>184</v>
       </c>
@@ -4974,7 +5026,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="189" spans="1:7">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="2"/>
       <c r="B189" s="2"/>
       <c r="C189" t="s">
@@ -4987,7 +5039,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="190" spans="1:7">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
         <v>185</v>
       </c>
@@ -5002,7 +5054,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="191" spans="1:7">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
         <v>186</v>
       </c>
@@ -5017,7 +5069,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="192" spans="1:7">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
         <v>187</v>
       </c>
@@ -5032,7 +5084,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="193" spans="1:7">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
         <v>188</v>
       </c>
@@ -5047,7 +5099,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="194" spans="1:7">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
         <v>189</v>
       </c>
@@ -5062,7 +5114,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="195" spans="1:7">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
         <v>190</v>
       </c>
@@ -5077,7 +5129,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="196" spans="1:7">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
         <v>191</v>
       </c>
@@ -5092,7 +5144,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="197" spans="1:7">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
         <v>192</v>
       </c>
@@ -5107,7 +5159,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="198" spans="1:7">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
         <v>193</v>
       </c>
@@ -5122,7 +5174,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="199" spans="1:7">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
         <v>194</v>
       </c>
@@ -5137,7 +5189,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="200" spans="1:7">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
         <v>195</v>
       </c>
@@ -5152,7 +5204,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="201" spans="1:7">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
         <v>196</v>
       </c>
@@ -5167,7 +5219,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="202" spans="1:7">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
         <v>197</v>
       </c>
@@ -5182,7 +5234,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="203" spans="1:7">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
         <v>198</v>
       </c>
@@ -5197,7 +5249,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="204" spans="1:7">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
         <v>199</v>
       </c>
@@ -5212,7 +5264,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="205" spans="1:7">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
         <v>200</v>
       </c>
@@ -5227,7 +5279,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="206" spans="1:7">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
         <v>201</v>
       </c>
@@ -5242,7 +5294,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="207" spans="1:7">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
         <v>202</v>
       </c>
@@ -5257,7 +5309,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="208" spans="1:7">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
         <v>203</v>
       </c>
@@ -5272,7 +5324,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="209" spans="1:7">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
         <v>204</v>
       </c>
@@ -5287,7 +5339,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="210" spans="1:7">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
         <v>205</v>
       </c>
@@ -5302,7 +5354,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="211" spans="1:7">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
         <v>206</v>
       </c>
@@ -5317,7 +5369,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="212" spans="1:7">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
         <v>207</v>
       </c>
@@ -5332,7 +5384,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="213" spans="1:7">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="s">
         <v>208</v>
       </c>
@@ -5347,7 +5399,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="214" spans="1:7">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
         <v>209</v>
       </c>
@@ -5362,7 +5414,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="215" spans="1:7">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
         <v>210</v>
       </c>
@@ -5377,7 +5429,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="216" spans="1:7">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="2"/>
       <c r="B216" s="2"/>
       <c r="C216" t="s">
@@ -5390,7 +5442,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="217" spans="1:7">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
         <v>211</v>
       </c>
@@ -5405,7 +5457,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="218" spans="1:7">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
         <v>212</v>
       </c>
@@ -5420,7 +5472,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="219" spans="1:7">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
         <v>213</v>
       </c>
@@ -5435,7 +5487,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="220" spans="1:7">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
         <v>214</v>
       </c>
@@ -5450,7 +5502,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="221" spans="1:7">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
         <v>215</v>
       </c>
@@ -5465,7 +5517,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="222" spans="1:7">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
         <v>216</v>
       </c>
@@ -5480,7 +5532,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="223" spans="1:7">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
         <v>217</v>
       </c>
@@ -5495,7 +5547,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="224" spans="1:7">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
         <v>218</v>
       </c>
@@ -5510,7 +5562,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="225" spans="1:7">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
         <v>219</v>
       </c>
@@ -5525,7 +5577,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="226" spans="1:7">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
         <v>220</v>
       </c>
@@ -5540,7 +5592,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="227" spans="1:7">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
         <v>221</v>
       </c>
@@ -5555,7 +5607,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="228" spans="1:7">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
         <v>222</v>
       </c>
@@ -5570,7 +5622,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="229" spans="1:7">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
         <v>223</v>
       </c>
@@ -5585,7 +5637,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="230" spans="1:7">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
         <v>224</v>
       </c>
@@ -5600,7 +5652,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="231" spans="1:7">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
         <v>225</v>
       </c>
@@ -5615,7 +5667,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="232" spans="1:7">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
         <v>226</v>
       </c>
@@ -5630,7 +5682,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="233" spans="1:7">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
         <v>227</v>
       </c>
@@ -5645,7 +5697,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="234" spans="1:7">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
         <v>228</v>
       </c>
@@ -5660,7 +5712,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="235" spans="1:7">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="s">
         <v>229</v>
       </c>
@@ -5675,7 +5727,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="236" spans="1:7">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="3" t="s">
         <v>230</v>
       </c>
@@ -5690,7 +5742,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="237" spans="1:7">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="3" t="s">
         <v>231</v>
       </c>
@@ -5705,7 +5757,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="238" spans="1:7">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="3" t="s">
         <v>232</v>
       </c>
@@ -5720,7 +5772,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="239" spans="1:7">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="3" t="s">
         <v>233</v>
       </c>
@@ -5735,7 +5787,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="240" spans="1:7">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="3" t="s">
         <v>234</v>
       </c>
@@ -5750,7 +5802,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="241" spans="1:7">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="3" t="s">
         <v>235</v>
       </c>
@@ -5765,7 +5817,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="242" spans="1:7">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="s">
         <v>236</v>
       </c>
@@ -5780,7 +5832,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="243" spans="1:7">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="3" t="s">
         <v>237</v>
       </c>
@@ -5795,7 +5847,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="244" spans="1:7">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="3" t="s">
         <v>238</v>
       </c>
@@ -5810,7 +5862,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="245" spans="1:7">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="3" t="s">
         <v>239</v>
       </c>
@@ -5825,7 +5877,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="246" spans="1:7">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" s="3" t="s">
         <v>240</v>
       </c>
@@ -5840,7 +5892,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="247" spans="1:7">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="2"/>
       <c r="B247" s="2"/>
       <c r="C247" t="s">
@@ -5853,7 +5905,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="248" spans="1:7">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="3" t="s">
         <v>241</v>
       </c>
@@ -5868,7 +5920,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="249" spans="1:7">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="3" t="s">
         <v>242</v>
       </c>
@@ -5883,7 +5935,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="250" spans="1:7">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="3" t="s">
         <v>243</v>
       </c>
@@ -5898,7 +5950,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="251" spans="1:7">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" s="3" t="s">
         <v>244</v>
       </c>
@@ -5913,7 +5965,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="252" spans="1:7">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" s="3" t="s">
         <v>245</v>
       </c>
@@ -5928,7 +5980,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="253" spans="1:7">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" s="3" t="s">
         <v>246</v>
       </c>
@@ -5943,7 +5995,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="254" spans="1:7">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="3" t="s">
         <v>247</v>
       </c>
@@ -5958,7 +6010,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="255" spans="1:7">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" s="3" t="s">
         <v>248</v>
       </c>
@@ -5973,7 +6025,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="256" spans="1:7">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" s="3" t="s">
         <v>249</v>
       </c>
@@ -5988,7 +6040,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="257" spans="1:7">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" s="3" t="s">
         <v>250</v>
       </c>
@@ -6003,7 +6055,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="258" spans="1:7">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A258" s="3" t="s">
         <v>251</v>
       </c>
@@ -6018,7 +6070,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="259" spans="1:7">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A259" s="3" t="s">
         <v>252</v>
       </c>
@@ -6033,7 +6085,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="260" spans="1:7">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A260" s="3" t="s">
         <v>253</v>
       </c>
@@ -6048,7 +6100,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="261" spans="1:7">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A261" s="3" t="s">
         <v>254</v>
       </c>
@@ -6063,7 +6115,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="262" spans="1:7">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A262" s="3" t="s">
         <v>255</v>
       </c>
@@ -6078,7 +6130,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="263" spans="1:7">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A263" s="3" t="s">
         <v>256</v>
       </c>
@@ -6093,7 +6145,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="264" spans="1:7">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A264" s="3" t="s">
         <v>257</v>
       </c>
@@ -6108,7 +6160,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="265" spans="1:7">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A265" s="3" t="s">
         <v>258</v>
       </c>
@@ -6123,7 +6175,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="266" spans="1:7">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A266" s="3" t="s">
         <v>259</v>
       </c>
@@ -6138,7 +6190,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="267" spans="1:7">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A267" s="3" t="s">
         <v>260</v>
       </c>
@@ -6153,7 +6205,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="268" spans="1:7">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A268" s="3" t="s">
         <v>261</v>
       </c>
@@ -6168,7 +6220,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="269" spans="1:7">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A269" s="3" t="s">
         <v>262</v>
       </c>
@@ -6183,7 +6235,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="270" spans="1:7">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A270" s="3" t="s">
         <v>263</v>
       </c>
@@ -6198,7 +6250,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="271" spans="1:7">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A271" s="3" t="s">
         <v>264</v>
       </c>
@@ -6213,7 +6265,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="272" spans="1:7">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A272" s="2"/>
       <c r="B272" s="2"/>
       <c r="C272" t="s">
@@ -6226,7 +6278,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="273" spans="1:7">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A273" s="3" t="s">
         <v>265</v>
       </c>
@@ -6241,7 +6293,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="274" spans="1:7">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A274" s="2"/>
       <c r="B274" s="2"/>
       <c r="C274" t="s">
@@ -6254,7 +6306,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="275" spans="1:7">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A275" s="3" t="s">
         <v>266</v>
       </c>
@@ -6269,7 +6321,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="276" spans="1:7">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A276" s="3" t="s">
         <v>267</v>
       </c>
@@ -6284,7 +6336,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="277" spans="1:7">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A277" s="3" t="s">
         <v>268</v>
       </c>
@@ -6299,7 +6351,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="278" spans="1:7">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A278" s="3" t="s">
         <v>269</v>
       </c>
@@ -6314,7 +6366,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="279" spans="1:7">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" s="3" t="s">
         <v>270</v>
       </c>
@@ -6329,7 +6381,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="280" spans="1:7">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A280" s="3" t="s">
         <v>271</v>
       </c>
@@ -6344,7 +6396,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="281" spans="1:7">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A281" s="3" t="s">
         <v>272</v>
       </c>
@@ -6359,7 +6411,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="282" spans="1:7">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A282" s="3" t="s">
         <v>273</v>
       </c>
@@ -6374,7 +6426,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="283" spans="1:7">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A283" s="3" t="s">
         <v>274</v>
       </c>
@@ -6389,7 +6441,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="284" spans="1:7">
+    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A284" s="3" t="s">
         <v>275</v>
       </c>
@@ -6404,7 +6456,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="285" spans="1:7">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A285" s="3" t="s">
         <v>276</v>
       </c>
@@ -6419,7 +6471,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="286" spans="1:7">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A286" s="3" t="s">
         <v>277</v>
       </c>
@@ -6434,7 +6486,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="287" spans="1:7">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A287" s="3" t="s">
         <v>278</v>
       </c>
@@ -6449,7 +6501,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="288" spans="1:7">
+    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A288" s="3" t="s">
         <v>279</v>
       </c>
@@ -6464,7 +6516,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="289" spans="1:7">
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A289" s="3" t="s">
         <v>280</v>
       </c>
@@ -6479,7 +6531,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="290" spans="1:7">
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A290" s="3" t="s">
         <v>281</v>
       </c>
@@ -6494,7 +6546,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="291" spans="1:7">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A291" s="3" t="s">
         <v>282</v>
       </c>
@@ -6509,7 +6561,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="292" spans="1:7">
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A292" s="3" t="s">
         <v>283</v>
       </c>
@@ -6524,7 +6576,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="293" spans="1:7">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A293" s="3" t="s">
         <v>284</v>
       </c>
@@ -6539,7 +6591,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="294" spans="1:7">
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A294" s="3" t="s">
         <v>285</v>
       </c>
@@ -6554,7 +6606,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="295" spans="1:7">
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A295" s="3" t="s">
         <v>286</v>
       </c>
@@ -6569,7 +6621,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="296" spans="1:7">
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A296" s="3" t="s">
         <v>287</v>
       </c>
@@ -6584,7 +6636,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="297" spans="1:7">
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A297" s="3" t="s">
         <v>288</v>
       </c>
@@ -6599,7 +6651,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="298" spans="1:7">
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A298" s="3" t="s">
         <v>289</v>
       </c>
@@ -6614,7 +6666,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="299" spans="1:7">
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A299" s="3" t="s">
         <v>290</v>
       </c>
@@ -6629,7 +6681,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="300" spans="1:7">
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A300" s="3" t="s">
         <v>291</v>
       </c>
@@ -6644,7 +6696,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="301" spans="1:7">
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A301" s="3" t="s">
         <v>292</v>
       </c>
@@ -6659,7 +6711,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="302" spans="1:7">
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A302" s="3" t="s">
         <v>293</v>
       </c>
@@ -6674,7 +6726,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="303" spans="1:7">
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A303" s="3" t="s">
         <v>294</v>
       </c>
@@ -6689,7 +6741,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="304" spans="1:7">
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A304" s="3" t="s">
         <v>295</v>
       </c>
@@ -6704,7 +6756,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="305" spans="1:7">
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A305" s="3" t="s">
         <v>296</v>
       </c>
@@ -6719,7 +6771,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="306" spans="1:7">
+    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A306" s="3" t="s">
         <v>297</v>
       </c>
@@ -6734,7 +6786,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="307" spans="1:7">
+    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A307" s="3" t="s">
         <v>298</v>
       </c>
@@ -6749,7 +6801,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="308" spans="1:7">
+    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A308" s="3" t="s">
         <v>299</v>
       </c>
@@ -6764,7 +6816,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="309" spans="1:7">
+    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A309" s="3" t="s">
         <v>300</v>
       </c>
@@ -6779,7 +6831,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="310" spans="1:7">
+    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A310" s="3" t="s">
         <v>301</v>
       </c>
@@ -6794,7 +6846,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="311" spans="1:7">
+    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A311" s="3" t="s">
         <v>302</v>
       </c>
@@ -6809,7 +6861,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="312" spans="1:7">
+    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A312" s="3" t="s">
         <v>303</v>
       </c>
@@ -6824,7 +6876,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="313" spans="1:7">
+    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A313" s="3" t="s">
         <v>304</v>
       </c>
@@ -6839,7 +6891,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="314" spans="1:7" ht="28">
+    <row r="314" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A314" s="3" t="s">
         <v>305</v>
       </c>
@@ -6854,7 +6906,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="315" spans="1:7">
+    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A315" s="3" t="s">
         <v>306</v>
       </c>
@@ -6869,7 +6921,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="316" spans="1:7">
+    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A316" s="3" t="s">
         <v>307</v>
       </c>
@@ -6884,7 +6936,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="317" spans="1:7">
+    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A317" s="3" t="s">
         <v>308</v>
       </c>
@@ -6899,7 +6951,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="318" spans="1:7">
+    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A318" s="3" t="s">
         <v>309</v>
       </c>
@@ -6914,7 +6966,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="319" spans="1:7">
+    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A319" s="3" t="s">
         <v>310</v>
       </c>
@@ -6929,7 +6981,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="320" spans="1:7">
+    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A320" s="3" t="s">
         <v>311</v>
       </c>
@@ -6944,7 +6996,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="321" spans="1:7">
+    <row r="321" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A321" s="3" t="s">
         <v>312</v>
       </c>
@@ -6959,7 +7011,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="322" spans="1:7">
+    <row r="322" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A322" s="3" t="s">
         <v>313</v>
       </c>
@@ -6974,7 +7026,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="323" spans="1:7">
+    <row r="323" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A323" s="3" t="s">
         <v>314</v>
       </c>
@@ -6989,7 +7041,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="324" spans="1:7">
+    <row r="324" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A324" s="3" t="s">
         <v>315</v>
       </c>
@@ -7004,7 +7056,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="325" spans="1:7">
+    <row r="325" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A325" s="3" t="s">
         <v>316</v>
       </c>
@@ -7019,7 +7071,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="326" spans="1:7">
+    <row r="326" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A326" s="3" t="s">
         <v>317</v>
       </c>
@@ -7034,7 +7086,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="327" spans="1:7">
+    <row r="327" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A327" s="3" t="s">
         <v>318</v>
       </c>
@@ -7049,7 +7101,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="328" spans="1:7">
+    <row r="328" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A328" s="3" t="s">
         <v>319</v>
       </c>
@@ -7064,7 +7116,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="329" spans="1:7">
+    <row r="329" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A329" s="3" t="s">
         <v>320</v>
       </c>
@@ -7079,7 +7131,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="330" spans="1:7">
+    <row r="330" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A330" s="3" t="s">
         <v>321</v>
       </c>
@@ -7094,7 +7146,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="331" spans="1:7">
+    <row r="331" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A331" s="3" t="s">
         <v>322</v>
       </c>
@@ -7109,7 +7161,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="332" spans="1:7">
+    <row r="332" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A332" s="3" t="s">
         <v>323</v>
       </c>
@@ -7124,7 +7176,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="333" spans="1:7">
+    <row r="333" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A333" s="3" t="s">
         <v>324</v>
       </c>
@@ -7139,7 +7191,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="334" spans="1:7">
+    <row r="334" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A334" s="3" t="s">
         <v>325</v>
       </c>
@@ -7154,7 +7206,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="335" spans="1:7">
+    <row r="335" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A335" s="3" t="s">
         <v>326</v>
       </c>
@@ -7169,7 +7221,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="336" spans="1:7">
+    <row r="336" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A336" s="3" t="s">
         <v>327</v>
       </c>
@@ -7184,7 +7236,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="337" spans="1:7">
+    <row r="337" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A337" s="3" t="s">
         <v>328</v>
       </c>
@@ -7199,7 +7251,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="338" spans="1:7">
+    <row r="338" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A338" s="3" t="s">
         <v>329</v>
       </c>
@@ -7214,7 +7266,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="339" spans="1:7">
+    <row r="339" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A339" s="3" t="s">
         <v>330</v>
       </c>
@@ -7229,7 +7281,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="340" spans="1:7">
+    <row r="340" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A340" s="3" t="s">
         <v>331</v>
       </c>
@@ -7244,7 +7296,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="341" spans="1:7">
+    <row r="341" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A341" s="3" t="s">
         <v>332</v>
       </c>
@@ -7259,7 +7311,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="342" spans="1:7">
+    <row r="342" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A342" s="3" t="s">
         <v>333</v>
       </c>
@@ -7274,7 +7326,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="343" spans="1:7">
+    <row r="343" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A343" s="3" t="s">
         <v>334</v>
       </c>
@@ -7289,7 +7341,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="344" spans="1:7">
+    <row r="344" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A344" s="3" t="s">
         <v>335</v>
       </c>
@@ -7304,7 +7356,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="345" spans="1:7">
+    <row r="345" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A345" s="3" t="s">
         <v>336</v>
       </c>
@@ -7319,7 +7371,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="346" spans="1:7">
+    <row r="346" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A346" s="3" t="s">
         <v>337</v>
       </c>
@@ -7334,7 +7386,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="347" spans="1:7">
+    <row r="347" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A347" s="3" t="s">
         <v>338</v>
       </c>
@@ -7349,7 +7401,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="348" spans="1:7">
+    <row r="348" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A348" s="3" t="s">
         <v>339</v>
       </c>
@@ -7364,7 +7416,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="349" spans="1:7">
+    <row r="349" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A349" s="3" t="s">
         <v>340</v>
       </c>
@@ -7379,7 +7431,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="350" spans="1:7">
+    <row r="350" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A350" s="3" t="s">
         <v>341</v>
       </c>
@@ -7394,7 +7446,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="351" spans="1:7">
+    <row r="351" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A351" s="3" t="s">
         <v>342</v>
       </c>
@@ -7409,7 +7461,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="352" spans="1:7">
+    <row r="352" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A352" s="3" t="s">
         <v>343</v>
       </c>
@@ -7424,7 +7476,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="353" spans="1:7">
+    <row r="353" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A353" s="3" t="s">
         <v>344</v>
       </c>
@@ -7439,7 +7491,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="354" spans="1:7">
+    <row r="354" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A354" s="3" t="s">
         <v>345</v>
       </c>
@@ -7454,7 +7506,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="355" spans="1:7">
+    <row r="355" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A355" s="3" t="s">
         <v>346</v>
       </c>
@@ -7469,7 +7521,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="356" spans="1:7">
+    <row r="356" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A356" s="3" t="s">
         <v>347</v>
       </c>
@@ -7484,7 +7536,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="357" spans="1:7">
+    <row r="357" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A357" s="3" t="s">
         <v>348</v>
       </c>
@@ -7499,7 +7551,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="358" spans="1:7">
+    <row r="358" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A358" s="3" t="s">
         <v>349</v>
       </c>
@@ -7514,7 +7566,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="359" spans="1:7">
+    <row r="359" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A359" s="3" t="s">
         <v>350</v>
       </c>
@@ -7529,7 +7581,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="360" spans="1:7">
+    <row r="360" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A360" s="3" t="s">
         <v>351</v>
       </c>
@@ -7544,7 +7596,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="361" spans="1:7">
+    <row r="361" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A361" s="3" t="s">
         <v>352</v>
       </c>
@@ -7559,7 +7611,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="362" spans="1:7">
+    <row r="362" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A362" s="3" t="s">
         <v>353</v>
       </c>
@@ -7574,7 +7626,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="363" spans="1:7">
+    <row r="363" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A363" s="3" t="s">
         <v>354</v>
       </c>
@@ -7589,7 +7641,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="364" spans="1:7">
+    <row r="364" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A364" s="3" t="s">
         <v>355</v>
       </c>
@@ -7603,8 +7655,11 @@
       <c r="G364" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="365" spans="1:7">
+      <c r="Q364" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="365" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A365" s="3" t="s">
         <v>356</v>
       </c>
@@ -7612,14 +7667,20 @@
       <c r="C365" t="s">
         <v>364</v>
       </c>
+      <c r="D365" s="7" t="s">
+        <v>448</v>
+      </c>
       <c r="E365" t="s">
         <v>367</v>
       </c>
+      <c r="F365" t="s">
+        <v>449</v>
+      </c>
       <c r="G365" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="366" spans="1:7">
+    <row r="366" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A366" s="3" t="s">
         <v>357</v>
       </c>
@@ -7627,6 +7688,9 @@
       <c r="C366" t="s">
         <v>364</v>
       </c>
+      <c r="D366" t="s">
+        <v>447</v>
+      </c>
       <c r="E366" t="s">
         <v>367</v>
       </c>
@@ -7634,7 +7698,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="367" spans="1:7">
+    <row r="367" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A367" s="3" t="s">
         <v>358</v>
       </c>
@@ -7642,38 +7706,50 @@
       <c r="C367" t="s">
         <v>364</v>
       </c>
+      <c r="D367" t="s">
+        <v>443</v>
+      </c>
       <c r="E367" t="s">
         <v>367</v>
       </c>
       <c r="G367" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="369" spans="1:2">
+      <c r="H367" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="Q367" t="s">
+        <v>442</v>
+      </c>
+      <c r="R367" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A369" s="4" t="s">
         <v>359</v>
       </c>
       <c r="B369" s="4"/>
     </row>
-    <row r="370" spans="1:2">
+    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370" s="4" t="s">
         <v>360</v>
       </c>
       <c r="B370" s="4"/>
     </row>
-    <row r="371" spans="1:2">
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" s="4" t="s">
         <v>361</v>
       </c>
       <c r="B371" s="4"/>
     </row>
-    <row r="372" spans="1:2">
+    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" s="4" t="s">
         <v>362</v>
       </c>
       <c r="B372" s="4"/>
     </row>
-    <row r="373" spans="1:2">
+    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" s="4" t="s">
         <v>363</v>
       </c>
@@ -7681,6 +7757,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:A373"/>
+  <hyperlinks>
+    <hyperlink ref="H367" r:id="rId1" display="http://moderntimesberlin.com/achive/&lt;number&gt;.jpg"/>
+    <hyperlink ref="D365" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>